<commit_message>
correccion recurso 20 tema 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC10.xlsx
+++ b/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC10.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="165">
   <si>
     <t>Fecha:</t>
   </si>
@@ -565,6 +565,9 @@
   </si>
   <si>
     <t>MA_11_02_REC10</t>
+  </si>
+  <si>
+    <t>Ocultar los puntos A, B, C, D</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,6 +769,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1270,7 +1285,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1325,9 +1340,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1449,16 +1461,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="9" borderId="5" xfId="51" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1543,6 +1568,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -2819,9 +2862,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2849,8 +2892,8 @@
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
@@ -2859,16 +2902,16 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="F2" s="73" t="s">
+      <c r="D2" s="85"/>
+      <c r="F2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2876,14 +2919,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="86">
         <v>11</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="D3" s="87"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -2891,19 +2934,19 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="86" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
@@ -2912,20 +2955,20 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="88" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="89"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="41" t="str">
+      <c r="F5" s="40" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
         <v>Motor del recurso</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="65"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
@@ -2937,20 +2980,20 @@
       <c r="E6" s="7"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="1"/>
@@ -2966,12 +3009,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="79"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2981,7 +3024,7 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -2996,16 +3039,16 @@
       <c r="E9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="H9" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="63" t="s">
         <v>121</v>
       </c>
       <c r="J9" s="20" t="s">
@@ -3016,79 +3059,79 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="12" customFormat="1" ht="233.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="str">
+      <c r="A10" s="69" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="75" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="22" t="str">
+      <c r="C10" s="71" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="14" t="str">
+      <c r="F10" s="72" t="str">
         <f t="shared" ref="F10:F13" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC10_IMG01n.png</v>
       </c>
-      <c r="G10" s="14" t="str">
+      <c r="G10" s="72" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H10" s="14" t="str">
+      <c r="H10" s="72" t="str">
         <f t="shared" ref="H10:H12" si="1">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC10_IMG01a.png</v>
       </c>
-      <c r="I10" s="14" t="str">
+      <c r="I10" s="72" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="71" t="s">
+      <c r="J10" s="72"/>
+      <c r="K10" s="74" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="12" customFormat="1" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="22" t="str">
+      <c r="C11" s="71" t="str">
         <f t="shared" ref="C11:C13" si="2">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="14" t="str">
+      <c r="F11" s="72" t="str">
         <f t="shared" si="0"/>
         <v>MA_11_02_REC10_IMG02n.png</v>
       </c>
-      <c r="G11" s="14" t="str">
+      <c r="G11" s="72" t="str">
         <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H11" s="14" t="str">
+      <c r="H11" s="72" t="str">
         <f t="shared" si="1"/>
         <v>MA_11_02_REC10_IMG02a.png</v>
       </c>
-      <c r="I11" s="14" t="str">
+      <c r="I11" s="72" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="71" t="s">
+      <c r="J11" s="72"/>
+      <c r="K11" s="74" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3125,226 +3168,228 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70" t="s">
+      <c r="J12" s="67"/>
+      <c r="K12" s="68" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="70" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="22" t="str">
+      <c r="C13" s="71" t="str">
         <f t="shared" si="2"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="14" t="str">
+      <c r="F13" s="72" t="str">
         <f t="shared" si="0"/>
         <v>MA_11_02_REC10_IMG04.png</v>
       </c>
-      <c r="G13" s="14" t="str">
+      <c r="G13" s="72" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13"/>
-      <c r="K13" s="71" t="s">
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="74" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="22" t="str">
+      <c r="C14" s="71" t="str">
         <f t="shared" ref="C14" si="3">IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="14" t="str">
+      <c r="F14" s="72" t="str">
         <f t="shared" ref="F14:F21" si="4">IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE($C$7,"_",$A14,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I14="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC10_IMG05n.png</v>
       </c>
-      <c r="G14" s="14" t="str">
+      <c r="G14" s="72" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H14" s="14" t="str">
+      <c r="H14" s="72" t="str">
         <f t="shared" ref="H14:H21" si="5">IF(AND(I14&lt;&gt;"",I14&lt;&gt;0),IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE($C$7,"_",$A14,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC10_IMG05a.png</v>
       </c>
-      <c r="I14" s="14" t="str">
+      <c r="I14" s="72" t="str">
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="72" t="s">
+      <c r="J14" s="72"/>
+      <c r="K14" s="108" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="275.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="110" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="22" t="str">
+      <c r="C15" s="110" t="str">
         <f t="shared" ref="C15" si="6">IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="111" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="111" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="14" t="str">
+      <c r="F15" s="111" t="str">
         <f t="shared" ref="F15" si="7">IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),CONCATENATE($C$7,"_",$A15,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I15="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC10_IMG06n.png</v>
       </c>
-      <c r="G15" s="14" t="str">
+      <c r="G15" s="111" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H15" s="14" t="str">
+      <c r="H15" s="111" t="str">
         <f t="shared" ref="H15" si="8">IF(AND(I15&lt;&gt;"",I15&lt;&gt;0),IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),CONCATENATE($C$7,"_",$A15,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC10_IMG06a.png</v>
       </c>
-      <c r="I15" s="14" t="str">
+      <c r="I15" s="111" t="str">
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
+      <c r="J15" s="111"/>
+      <c r="K15" s="112" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="C16" s="22" t="str">
+      <c r="C16" s="71" t="str">
         <f t="shared" ref="C16" si="9">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="14" t="str">
+      <c r="F16" s="72" t="str">
         <f t="shared" ref="F16" si="10">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE($C$7,"_",$A16,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I16="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC10_IMG07n.png</v>
       </c>
-      <c r="G16" s="14" t="str">
+      <c r="G16" s="72" t="str">
         <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H16" s="14" t="str">
+      <c r="H16" s="72" t="str">
         <f t="shared" ref="H16" si="11">IF(AND(I16&lt;&gt;"",I16&lt;&gt;0),IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE($C$7,"_",$A16,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC10_IMG07a.png</v>
       </c>
-      <c r="I16" s="14" t="str">
+      <c r="I16" s="72" t="str">
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="15"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="113"/>
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" ht="192" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="22" t="str">
+      <c r="C17" s="71" t="str">
         <f t="shared" ref="C17" si="12">IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="14" t="str">
+      <c r="F17" s="72" t="str">
         <f t="shared" ref="F17" si="13">IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A17,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I17="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC10_IMG08n.png</v>
       </c>
-      <c r="G17" s="14" t="str">
+      <c r="G17" s="72" t="str">
         <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H17" s="14" t="str">
+      <c r="H17" s="72" t="str">
         <f t="shared" ref="H17" si="14">IF(AND(I17&lt;&gt;"",I17&lt;&gt;0),IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A17,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC10_IMG08a.png</v>
       </c>
-      <c r="I17" s="14" t="str">
+      <c r="I17" s="72" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15" t="s">
+      <c r="J17" s="72"/>
+      <c r="K17" s="113" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="69" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="C18" s="22" t="str">
+      <c r="C18" s="71" t="str">
         <f t="shared" ref="C18" si="15">IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M5A</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F18" s="14" t="str">
+      <c r="F18" s="72" t="str">
         <f t="shared" ref="F18" si="16">IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),CONCATENATE($C$7,"_",$A18,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I18="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC10_IMG09n.png</v>
       </c>
-      <c r="G18" s="14" t="str">
+      <c r="G18" s="72" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>286 x 286 px</v>
       </c>
-      <c r="H18" s="14" t="str">
+      <c r="H18" s="72" t="str">
         <f t="shared" ref="H18" si="17">IF(AND(I18&lt;&gt;"",I18&lt;&gt;0),IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),CONCATENATE($C$7,"_",$A18,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC10_IMG09a.png</v>
       </c>
-      <c r="I18" s="14" t="str">
+      <c r="I18" s="72" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="113"/>
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
@@ -4766,539 +4811,539 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="26" customWidth="1"/>
-    <col min="2" max="2" width="11" style="26"/>
-    <col min="3" max="3" width="13.875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="26" customWidth="1"/>
-    <col min="5" max="7" width="11" style="26"/>
-    <col min="8" max="11" width="11" style="26" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="26"/>
+    <col min="1" max="1" width="72.25" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11" style="25"/>
+    <col min="3" max="3" width="13.875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="25" customWidth="1"/>
+    <col min="5" max="7" width="11" style="25"/>
+    <col min="8" max="11" width="11" style="25" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="90"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="94"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="91" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="97" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="98"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="36"/>
-      <c r="H3" s="26" t="s">
+      <c r="D3" s="102"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="35"/>
+      <c r="H3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="H4" s="26" t="s">
+      <c r="F4" s="35"/>
+      <c r="H4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <v>1</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="100" t="str">
+      <c r="D5" s="104" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>MA_11_01_CO</v>
       </c>
-      <c r="E5" s="101"/>
-      <c r="F5" s="36"/>
-      <c r="H5" s="26" t="s">
+      <c r="E5" s="105"/>
+      <c r="F5" s="35"/>
+      <c r="H5" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="25">
         <v>2</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
-      <c r="H6" s="26" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="H6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="25">
         <v>3</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="66" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="86" t="str">
+      <c r="D7" s="90" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_MA_11_01_CO.xls</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
-      <c r="H7" s="26" t="s">
+      <c r="E7" s="90"/>
+      <c r="F7" s="91"/>
+      <c r="H7" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <v>4</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="25">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
-      <c r="I8" s="26" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="I8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="25">
         <v>5</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="25">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
-      <c r="I9" s="26" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="I9" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="25">
         <v>6</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="25">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
-      <c r="I10" s="26" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
+      <c r="I10" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="25">
         <v>7</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="25">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="25">
         <v>8</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="25">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="26">
+      <c r="J12" s="25">
         <v>9</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="25">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="90"/>
-      <c r="I13" s="26" t="s">
+      <c r="B13" s="93"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="94"/>
+      <c r="I13" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="25">
         <v>10</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="25">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-      <c r="I14" s="26" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="I14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="25">
         <v>11</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="25">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="91" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="93"/>
-      <c r="J15" s="26">
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
+      <c r="J15" s="25">
         <v>12</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="25">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="30" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="25">
         <v>13</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="25">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="32" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="94" t="str">
+      <c r="D17" s="98" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>MA_11_01_REC10</v>
       </c>
-      <c r="E17" s="95"/>
-      <c r="F17" s="96"/>
-      <c r="J17" s="26">
+      <c r="E17" s="99"/>
+      <c r="F17" s="100"/>
+      <c r="J17" s="25">
         <v>14</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="25">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="66" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="86" t="str">
+      <c r="D18" s="90" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_MA_11_01_REC10.xls</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="87"/>
-      <c r="J18" s="26">
+      <c r="E18" s="90"/>
+      <c r="F18" s="91"/>
+      <c r="J18" s="25">
         <v>15</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="25">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-      <c r="H19" s="26">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="H19" s="25">
         <v>3</v>
       </c>
-      <c r="J19" s="26">
+      <c r="J19" s="25">
         <v>16</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="25">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="H20" s="26">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
+      <c r="H20" s="25">
         <v>1</v>
       </c>
-      <c r="I20" s="26">
+      <c r="I20" s="25">
         <v>9</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20" s="25">
         <v>1</v>
       </c>
-      <c r="K20" s="26">
+      <c r="K20" s="25">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H21" s="26" t="str">
+      <c r="H21" s="25" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>MA</v>
       </c>
-      <c r="I21" s="26" t="str">
+      <c r="I21" s="25" t="str">
         <f>CONCATENATE(IF((I20+2)&lt;10,"0",""),I20+2)</f>
         <v>11</v>
       </c>
-      <c r="J21" s="26" t="str">
+      <c r="J21" s="25" t="str">
         <f>CONCATENATE(IF(J20&lt;10,"0",""),J20)</f>
         <v>01</v>
       </c>
-      <c r="K21" s="26">
+      <c r="K21" s="25">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K22" s="26">
+      <c r="K22" s="25">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K23" s="26">
+      <c r="K23" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K24" s="26">
+      <c r="K24" s="25">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K25" s="26">
+      <c r="K25" s="25">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K26" s="26">
+      <c r="K26" s="25">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K27" s="26">
+      <c r="K27" s="25">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K28" s="26">
+      <c r="K28" s="25">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K29" s="26">
+      <c r="K29" s="25">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K30" s="26">
+      <c r="K30" s="25">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K31" s="26">
+      <c r="K31" s="25">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K32" s="26">
+      <c r="K32" s="25">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="26">
+      <c r="K33" s="25">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K34" s="26">
+      <c r="K34" s="25">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K35" s="26">
+      <c r="K35" s="25">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K36" s="26">
+      <c r="K36" s="25">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K37" s="26">
+      <c r="K37" s="25">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K38" s="26">
+      <c r="K38" s="25">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K39" s="26">
+      <c r="K39" s="25">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K40" s="26">
+      <c r="K40" s="25">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K41" s="26">
+      <c r="K41" s="25">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K42" s="26">
+      <c r="K42" s="25">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K43" s="26">
+      <c r="K43" s="25">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K44" s="26">
+      <c r="K44" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K45" s="26" t="str">
+      <c r="K45" s="25" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
       </c>
@@ -5493,562 +5538,562 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="26" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="26" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="26"/>
-    <col min="5" max="5" width="11.75" style="26" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="26" customWidth="1"/>
-    <col min="7" max="7" width="11" style="26" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="26" customWidth="1"/>
-    <col min="9" max="9" width="22.25" style="26" customWidth="1"/>
-    <col min="10" max="10" width="20.75" style="26" customWidth="1"/>
-    <col min="11" max="11" width="44.5" style="26" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="26"/>
+    <col min="1" max="1" width="21" style="25" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="25"/>
+    <col min="5" max="5" width="11.75" style="25" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="25" customWidth="1"/>
+    <col min="7" max="7" width="11" style="25" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="25" customWidth="1"/>
+    <col min="9" max="9" width="22.25" style="25" customWidth="1"/>
+    <col min="10" max="10" width="20.75" style="25" customWidth="1"/>
+    <col min="11" max="11" width="44.5" style="25" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="102"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="45" t="s">
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-    </row>
-    <row r="4" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+    </row>
+    <row r="4" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="48"/>
-    </row>
-    <row r="5" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="J4" s="47"/>
+    </row>
+    <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="48" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J5" s="50"/>
-    </row>
-    <row r="6" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="J5" s="49"/>
+    </row>
+    <row r="6" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J6" s="48" t="s">
+      <c r="J6" s="47" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="47" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:11" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J7" s="48"/>
-    </row>
-    <row r="8" spans="1:11" s="47" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="J7" s="47"/>
+    </row>
+    <row r="8" spans="1:11" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48" t="s">
+      <c r="G8" s="47"/>
+      <c r="H8" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J8" s="48"/>
-    </row>
-    <row r="9" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="J8" s="47"/>
+    </row>
+    <row r="9" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48" t="s">
+      <c r="G9" s="47"/>
+      <c r="H9" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J9" s="48"/>
-    </row>
-    <row r="10" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="J9" s="47"/>
+    </row>
+    <row r="10" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48" t="s">
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J10" s="48"/>
-    </row>
-    <row r="11" spans="1:11" s="47" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="J10" s="47"/>
+    </row>
+    <row r="11" spans="1:11" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48" t="s">
+      <c r="G11" s="47"/>
+      <c r="H11" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J11" s="48"/>
-    </row>
-    <row r="12" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="J11" s="47"/>
+    </row>
+    <row r="12" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48" t="s">
+      <c r="G12" s="47"/>
+      <c r="H12" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I12" s="48" t="s">
+      <c r="I12" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J12" s="48"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53" t="s">
+      <c r="E13" s="51"/>
+      <c r="F13" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48" t="s">
+      <c r="G13" s="50"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="J13" s="51"/>
-      <c r="K13" s="26" t="s">
+      <c r="J13" s="50"/>
+      <c r="K13" s="25" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53" t="s">
+      <c r="E14" s="51"/>
+      <c r="F14" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="G14" s="51"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48" t="s">
+      <c r="G14" s="50"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="J14" s="51"/>
+      <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="51" t="s">
+      <c r="E15" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="48" t="s">
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="26" t="s">
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="25" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="49" t="s">
+      <c r="B16" s="52"/>
+      <c r="C16" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="53" t="s">
+      <c r="D16" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="52" t="s">
+      <c r="F16" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53" t="s">
+      <c r="G16" s="51"/>
+      <c r="H16" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="I16" s="53" t="s">
+      <c r="I16" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="52"/>
-      <c r="K16" s="54" t="s">
+      <c r="J16" s="51"/>
+      <c r="K16" s="53" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="55" t="s">
+      <c r="G17" s="47"/>
+      <c r="H17" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="I17" s="55" t="s">
+      <c r="I17" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="J17" s="48"/>
-      <c r="K17" s="56" t="s">
+      <c r="J17" s="47"/>
+      <c r="K17" s="55" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
     </row>
     <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="C24" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C25" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
     </row>
     <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>